<commit_message>
Updated formula on spreadsheet.
</commit_message>
<xml_diff>
--- a/spreadsheets/Chapter01-bus-times.xlsx
+++ b/spreadsheets/Chapter01-bus-times.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\__Projetos\__TODO\Books-writing\2022\Markov Chains primer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stout\Google Drive\__Projetos\__TODO\Books-writing\2022\Markov Chains primer\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4AE2E1-B9A0-4FA4-BD1B-DF91F64DA4A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0633B9D5-BCAE-4740-83C8-67604FF89945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Time waiting for a bus" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>December</t>
   </si>
   <si>
-    <t>Formula used: '=(-$C$1)*LN(1-RAND()) -- convert from uniform to exponential distribution</t>
-  </si>
-  <si>
     <t>Mean:</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>Parameter</t>
+  </si>
+  <si>
+    <t>Formula used: '=(-1/$C$1)*LN(1-RAND()) -- convert from uniform to exponential distribution</t>
   </si>
 </sst>
 </file>
@@ -7502,31 +7502,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="14" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1">
         <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="F1" s="19"/>
       <c r="G1" s="19"/>
@@ -7543,10 +7545,10 @@
       <c r="R1" s="19"/>
       <c r="S1" s="19"/>
     </row>
-    <row r="2" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:20" ht="57.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="55.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
@@ -7587,7 +7589,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" s="7">
         <v>1</v>
       </c>
@@ -7628,17 +7630,17 @@
         <v>1.45806122409854</v>
       </c>
       <c r="P4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Q4" s="2">
         <f>AVERAGE(C4:N34)</f>
         <v>21.6983655462858</v>
       </c>
       <c r="R4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B5" s="8">
         <v>2</v>
       </c>
@@ -7679,24 +7681,24 @@
         <v>39.554217957038119</v>
       </c>
       <c r="P5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q5" s="2">
         <f>MIN(C4:N34)</f>
         <v>5.3036010963462416E-2</v>
       </c>
       <c r="R5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S5" s="2">
         <f>Q5*60</f>
         <v>3.1821606578077448</v>
       </c>
       <c r="T5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B6" s="8">
         <v>3</v>
       </c>
@@ -7737,24 +7739,24 @@
         <v>11.840412452268405</v>
       </c>
       <c r="P6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q6" s="2">
         <f>MAX(C4:N34)</f>
         <v>148.53511309673706</v>
       </c>
       <c r="R6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="S6" s="2">
         <f>Q6/60</f>
         <v>2.4755852182789511</v>
       </c>
       <c r="T6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B7" s="8">
         <v>4</v>
       </c>
@@ -7795,7 +7797,7 @@
         <v>24.59608852779537</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B8" s="8">
         <v>5</v>
       </c>
@@ -7836,7 +7838,7 @@
         <v>28.054075210901726</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B9" s="8">
         <v>6</v>
       </c>
@@ -7877,7 +7879,7 @@
         <v>11.353229153375061</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B10" s="8">
         <v>7</v>
       </c>
@@ -7918,7 +7920,7 @@
         <v>1.0322110167694853</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B11" s="8">
         <v>8</v>
       </c>
@@ -7959,7 +7961,7 @@
         <v>2.8854913637380712</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" s="8">
         <v>9</v>
       </c>
@@ -8000,7 +8002,7 @@
         <v>40.265426649196307</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B13" s="8">
         <v>10</v>
       </c>
@@ -8041,7 +8043,7 @@
         <v>12.686057605020956</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B14" s="8">
         <v>11</v>
       </c>
@@ -8082,7 +8084,7 @@
         <v>36.254631666230196</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B15" s="8">
         <v>12</v>
       </c>
@@ -8123,7 +8125,7 @@
         <v>0.2406594522544582</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B16" s="8">
         <v>13</v>
       </c>
@@ -8164,7 +8166,7 @@
         <v>0.67575745758051808</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="8">
         <v>14</v>
       </c>
@@ -8205,7 +8207,7 @@
         <v>11.355695386724848</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" s="8">
         <v>15</v>
       </c>
@@ -8246,7 +8248,7 @@
         <v>17.324271536888908</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" s="8">
         <v>16</v>
       </c>
@@ -8287,7 +8289,7 @@
         <v>0.25806913929772085</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" s="8">
         <v>17</v>
       </c>
@@ -8328,7 +8330,7 @@
         <v>21.862649211279091</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="8">
         <v>18</v>
       </c>
@@ -8369,7 +8371,7 @@
         <v>5.0610730331095954</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="8">
         <v>19</v>
       </c>
@@ -8410,7 +8412,7 @@
         <v>49.466289247640923</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" s="8">
         <v>20</v>
       </c>
@@ -8451,7 +8453,7 @@
         <v>5.2189475071263729</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" s="8">
         <v>21</v>
       </c>
@@ -8492,7 +8494,7 @@
         <v>19.780650492844064</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" s="8">
         <v>22</v>
       </c>
@@ -8533,7 +8535,7 @@
         <v>40.454535435984518</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" s="8">
         <v>23</v>
       </c>
@@ -8574,7 +8576,7 @@
         <v>16.172666574789307</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" s="8">
         <v>24</v>
       </c>
@@ -8615,7 +8617,7 @@
         <v>55.463694636734914</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="8">
         <v>25</v>
       </c>
@@ -8656,7 +8658,7 @@
         <v>4.1112235772446954</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="8">
         <v>26</v>
       </c>
@@ -8697,7 +8699,7 @@
         <v>9.4523104498002706</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="8">
         <v>27</v>
       </c>
@@ -8738,7 +8740,7 @@
         <v>7.0521791099095568</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" s="8">
         <v>28</v>
       </c>
@@ -8779,7 +8781,7 @@
         <v>5.6233165502401743</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" s="8">
         <v>29</v>
       </c>
@@ -8818,7 +8820,7 @@
         <v>15.108317824582702</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" s="8">
         <v>30</v>
       </c>
@@ -8857,7 +8859,7 @@
         <v>20.61037891270038</v>
       </c>
     </row>
-    <row r="34" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="9">
         <v>31</v>
       </c>
@@ -8888,9 +8890,9 @@
         <v>22.225718444421769</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C35" s="2">
         <f>AVERAGE(C4:C34)</f>
@@ -8959,14 +8961,14 @@
       <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -8974,7 +8976,7 @@
         <v>5.3036010963462416E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -8982,7 +8984,7 @@
         <v>7.4565360669439862E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -8990,7 +8992,7 @@
         <v>0.2406594522544582</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -8998,7 +9000,7 @@
         <v>0.25806913929772085</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9006,7 +9008,7 @@
         <v>0.34294077826422525</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -9014,7 +9016,7 @@
         <v>0.36950848519128304</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -9022,7 +9024,7 @@
         <v>0.53351436300057875</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -9030,7 +9032,7 @@
         <v>0.67361159996795683</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -9038,7 +9040,7 @@
         <v>0.67575745758051808</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -9046,7 +9048,7 @@
         <v>0.68050238711728017</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -9054,7 +9056,7 @@
         <v>0.68233258480918124</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -9062,7 +9064,7 @@
         <v>0.97494390053003688</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -9070,7 +9072,7 @@
         <v>1.028746647221966</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -9078,7 +9080,7 @@
         <v>1.0322110167694853</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -9086,7 +9088,7 @@
         <v>1.0987952079018168</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -9094,7 +9096,7 @@
         <v>1.1943266944510396</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -9102,7 +9104,7 @@
         <v>1.2225578136054209</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -9110,7 +9112,7 @@
         <v>1.22294855149564</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -9118,7 +9120,7 @@
         <v>1.2707550499110345</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -9126,7 +9128,7 @@
         <v>1.3898013887312446</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -9134,7 +9136,7 @@
         <v>1.3960798671154167</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -9142,7 +9144,7 @@
         <v>1.45806122409854</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -9150,7 +9152,7 @@
         <v>1.530502404542238</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -9158,7 +9160,7 @@
         <v>1.5565081801924472</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -9166,7 +9168,7 @@
         <v>1.6185154793567413</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -9174,7 +9176,7 @@
         <v>1.6470591028742054</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -9182,7 +9184,7 @@
         <v>1.6964726394227307</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -9190,7 +9192,7 @@
         <v>1.7490878756652801</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -9198,7 +9200,7 @@
         <v>1.7883493286795915</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -9206,7 +9208,7 @@
         <v>1.98091881323583</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -9214,7 +9216,7 @@
         <v>1.9809808455456301</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -9222,7 +9224,7 @@
         <v>2.0128717138915238</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -9230,7 +9232,7 @@
         <v>2.1237779823298348</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -9238,7 +9240,7 @@
         <v>2.146095315335403</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -9246,7 +9248,7 @@
         <v>2.1534734655352836</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -9254,7 +9256,7 @@
         <v>2.1913982397259062</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -9262,7 +9264,7 @@
         <v>2.2579627900492678</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -9270,7 +9272,7 @@
         <v>2.2743850966228565</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -9278,7 +9280,7 @@
         <v>2.2878118622928092</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -9286,7 +9288,7 @@
         <v>2.3839013234963065</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -9294,7 +9296,7 @@
         <v>2.615002674614169</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -9302,7 +9304,7 @@
         <v>2.775409990368138</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -9310,7 +9312,7 @@
         <v>2.8559569304741022</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -9318,7 +9320,7 @@
         <v>2.8854913637380712</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -9326,7 +9328,7 @@
         <v>2.9177646426983763</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -9334,7 +9336,7 @@
         <v>2.9410055632362475</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -9342,7 +9344,7 @@
         <v>2.9900031919388264</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -9350,7 +9352,7 @@
         <v>3.0302950572106284</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -9358,7 +9360,7 @@
         <v>3.1059680520639632</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -9366,7 +9368,7 @@
         <v>3.1352711261374075</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -9374,7 +9376,7 @@
         <v>3.155119147033818</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -9382,7 +9384,7 @@
         <v>3.2502752515153599</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -9390,7 +9392,7 @@
         <v>3.265466616218176</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -9398,7 +9400,7 @@
         <v>3.4122842182623172</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -9406,7 +9408,7 @@
         <v>3.4139449505732933</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -9414,7 +9416,7 @@
         <v>3.4166624680757489</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -9422,7 +9424,7 @@
         <v>3.4320903354834882</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -9430,7 +9432,7 @@
         <v>3.4546197632157165</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -9438,7 +9440,7 @@
         <v>3.4781642599014564</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -9446,7 +9448,7 @@
         <v>3.5287623372553578</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -9454,7 +9456,7 @@
         <v>3.6440775448483995</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -9462,7 +9464,7 @@
         <v>3.9347458914289883</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -9470,7 +9472,7 @@
         <v>4.1112235772446954</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -9478,7 +9480,7 @@
         <v>4.1330783687644166</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
@@ -9486,7 +9488,7 @@
         <v>4.2346363470605883</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
@@ -9494,7 +9496,7 @@
         <v>4.3708921640091685</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
@@ -9502,7 +9504,7 @@
         <v>4.397676062973229</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
@@ -9510,7 +9512,7 @@
         <v>4.4061113951598392</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
@@ -9518,7 +9520,7 @@
         <v>4.4505799584565278</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
@@ -9526,7 +9528,7 @@
         <v>4.4816032579132994</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
@@ -9534,7 +9536,7 @@
         <v>4.589366349303444</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
@@ -9542,7 +9544,7 @@
         <v>4.6886698557011357</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
@@ -9550,7 +9552,7 @@
         <v>4.7050492316267976</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
@@ -9558,7 +9560,7 @@
         <v>4.7162563433185225</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
@@ -9566,7 +9568,7 @@
         <v>4.8742060401834832</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
@@ -9574,7 +9576,7 @@
         <v>4.90510114357535</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
@@ -9582,7 +9584,7 @@
         <v>4.9279532507407389</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
@@ -9590,7 +9592,7 @@
         <v>5.0462739530213412</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
@@ -9598,7 +9600,7 @@
         <v>5.0610730331095954</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
@@ -9606,7 +9608,7 @@
         <v>5.0738997156901613</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
@@ -9614,7 +9616,7 @@
         <v>5.1631494399893461</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
@@ -9622,7 +9624,7 @@
         <v>5.2189475071263729</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
@@ -9630,7 +9632,7 @@
         <v>5.2276910427668106</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
@@ -9638,7 +9640,7 @@
         <v>5.2955948095509564</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
@@ -9646,7 +9648,7 @@
         <v>5.3788609054891126</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
@@ -9654,7 +9656,7 @@
         <v>5.3917232176875141</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
@@ -9662,7 +9664,7 @@
         <v>5.448116597820448</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
@@ -9670,7 +9672,7 @@
         <v>5.520066288552167</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
@@ -9678,7 +9680,7 @@
         <v>5.6233165502401743</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
@@ -9686,7 +9688,7 @@
         <v>5.6411818479943863</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
@@ -9694,7 +9696,7 @@
         <v>5.690752181342539</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
@@ -9702,7 +9704,7 @@
         <v>5.718909441543393</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
@@ -9710,7 +9712,7 @@
         <v>5.7778581411799212</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
@@ -9718,7 +9720,7 @@
         <v>5.8543517993271017</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
@@ -9726,7 +9728,7 @@
         <v>5.8607758765514175</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
@@ -9734,7 +9736,7 @@
         <v>5.8939878499793572</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
@@ -9742,7 +9744,7 @@
         <v>5.9165589086005301</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
@@ -9750,7 +9752,7 @@
         <v>5.9878358390079987</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
@@ -9758,7 +9760,7 @@
         <v>5.9927544213443529</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
       </c>
@@ -9766,7 +9768,7 @@
         <v>6.0489013277397472</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>101</v>
       </c>
@@ -9774,7 +9776,7 @@
         <v>6.0804200884671129</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>102</v>
       </c>
@@ -9782,7 +9784,7 @@
         <v>6.1912598060096871</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>103</v>
       </c>
@@ -9790,7 +9792,7 @@
         <v>6.2423394667693985</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>104</v>
       </c>
@@ -9798,7 +9800,7 @@
         <v>6.2713042421233993</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>105</v>
       </c>
@@ -9806,7 +9808,7 @@
         <v>6.4098535038933599</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>106</v>
       </c>
@@ -9814,7 +9816,7 @@
         <v>6.5695647643015871</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>107</v>
       </c>
@@ -9822,7 +9824,7 @@
         <v>6.576036293548233</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>108</v>
       </c>
@@ -9830,7 +9832,7 @@
         <v>6.6682676053511276</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>109</v>
       </c>
@@ -9838,7 +9840,7 @@
         <v>6.6702448703929997</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>110</v>
       </c>
@@ -9846,7 +9848,7 @@
         <v>6.6957095656031154</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>111</v>
       </c>
@@ -9854,7 +9856,7 @@
         <v>6.7322436569185911</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -9862,7 +9864,7 @@
         <v>6.733924887615407</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -9870,7 +9872,7 @@
         <v>6.8043643307572808</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -9878,7 +9880,7 @@
         <v>6.8457939784895618</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -9886,7 +9888,7 @@
         <v>6.8892712894144825</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -9894,7 +9896,7 @@
         <v>6.969614667198746</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -9902,7 +9904,7 @@
         <v>7.0521791099095568</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -9910,7 +9912,7 @@
         <v>7.0589650424230452</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -9918,7 +9920,7 @@
         <v>7.3050149839956413</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -9926,7 +9928,7 @@
         <v>7.3064934379931028</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -9934,7 +9936,7 @@
         <v>7.3856182286128504</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -9942,7 +9944,7 @@
         <v>7.5389213309480843</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -9950,7 +9952,7 @@
         <v>7.566916402613745</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -9958,7 +9960,7 @@
         <v>8.1325729055880505</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -9966,7 +9968,7 @@
         <v>8.444799052428106</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -9974,7 +9976,7 @@
         <v>8.4739866261944279</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -9982,7 +9984,7 @@
         <v>8.534888033398742</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>128</v>
       </c>
@@ -9990,7 +9992,7 @@
         <v>8.6096946231160629</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>129</v>
       </c>
@@ -9998,7 +10000,7 @@
         <v>8.7293096481711014</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>130</v>
       </c>
@@ -10006,7 +10008,7 @@
         <v>8.7493427795602532</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>131</v>
       </c>
@@ -10014,7 +10016,7 @@
         <v>8.8127606093065722</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>132</v>
       </c>
@@ -10022,7 +10024,7 @@
         <v>9.0780524183350533</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>133</v>
       </c>
@@ -10030,7 +10032,7 @@
         <v>9.1416422843331961</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>134</v>
       </c>
@@ -10038,7 +10040,7 @@
         <v>9.2666623690081149</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>135</v>
       </c>
@@ -10046,7 +10048,7 @@
         <v>9.2839081500900704</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>136</v>
       </c>
@@ -10054,7 +10056,7 @@
         <v>9.4038403103316615</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>137</v>
       </c>
@@ -10062,7 +10064,7 @@
         <v>9.4523104498002706</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>138</v>
       </c>
@@ -10070,7 +10072,7 @@
         <v>9.5443363236886487</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>139</v>
       </c>
@@ -10078,7 +10080,7 @@
         <v>9.5830989804015374</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>140</v>
       </c>
@@ -10086,7 +10088,7 @@
         <v>9.632945097460599</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>141</v>
       </c>
@@ -10094,7 +10096,7 @@
         <v>9.752346550131886</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>142</v>
       </c>
@@ -10102,7 +10104,7 @@
         <v>9.8582415995052983</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>143</v>
       </c>
@@ -10110,7 +10112,7 @@
         <v>9.9291774386409504</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
@@ -10118,7 +10120,7 @@
         <v>10.080856832412856</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>145</v>
       </c>
@@ -10126,7 +10128,7 @@
         <v>10.091594866631972</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>146</v>
       </c>
@@ -10134,7 +10136,7 @@
         <v>10.107320137582199</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>147</v>
       </c>
@@ -10142,7 +10144,7 @@
         <v>10.197030192780694</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>148</v>
       </c>
@@ -10150,7 +10152,7 @@
         <v>10.20015305580282</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>149</v>
       </c>
@@ -10158,7 +10160,7 @@
         <v>10.217301954671058</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>150</v>
       </c>
@@ -10166,7 +10168,7 @@
         <v>10.283158840278288</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>151</v>
       </c>
@@ -10174,7 +10176,7 @@
         <v>10.426651150637989</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>152</v>
       </c>
@@ -10182,7 +10184,7 @@
         <v>10.58965954567541</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>153</v>
       </c>
@@ -10190,7 +10192,7 @@
         <v>10.593100191410866</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>154</v>
       </c>
@@ -10198,7 +10200,7 @@
         <v>10.600764896656257</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>155</v>
       </c>
@@ -10206,7 +10208,7 @@
         <v>10.856442243474724</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>156</v>
       </c>
@@ -10214,7 +10216,7 @@
         <v>10.968435898176146</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>157</v>
       </c>
@@ -10222,7 +10224,7 @@
         <v>11.149230741535852</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>158</v>
       </c>
@@ -10230,7 +10232,7 @@
         <v>11.171848321337814</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>159</v>
       </c>
@@ -10238,7 +10240,7 @@
         <v>11.19798519487688</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>160</v>
       </c>
@@ -10246,7 +10248,7 @@
         <v>11.230475086742914</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>161</v>
       </c>
@@ -10254,7 +10256,7 @@
         <v>11.353229153375061</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>162</v>
       </c>
@@ -10262,7 +10264,7 @@
         <v>11.355695386724848</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>163</v>
       </c>
@@ -10270,7 +10272,7 @@
         <v>11.593434915346151</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>164</v>
       </c>
@@ -10278,7 +10280,7 @@
         <v>11.743414996336446</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>165</v>
       </c>
@@ -10286,7 +10288,7 @@
         <v>11.840412452268405</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>166</v>
       </c>
@@ -10294,7 +10296,7 @@
         <v>11.971948752723907</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>167</v>
       </c>
@@ -10302,7 +10304,7 @@
         <v>12.194942206398409</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>168</v>
       </c>
@@ -10310,7 +10312,7 @@
         <v>12.209070233169166</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>169</v>
       </c>
@@ -10318,7 +10320,7 @@
         <v>12.294195682044148</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>170</v>
       </c>
@@ -10326,7 +10328,7 @@
         <v>12.686057605020956</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>171</v>
       </c>
@@ -10334,7 +10336,7 @@
         <v>12.924823645551752</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>172</v>
       </c>
@@ -10342,7 +10344,7 @@
         <v>12.94284327066589</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>173</v>
       </c>
@@ -10350,7 +10352,7 @@
         <v>13.005928941578439</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>174</v>
       </c>
@@ -10358,7 +10360,7 @@
         <v>13.222564937220806</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>175</v>
       </c>
@@ -10366,7 +10368,7 @@
         <v>13.238012475225315</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>176</v>
       </c>
@@ -10374,7 +10376,7 @@
         <v>13.415289362497989</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>177</v>
       </c>
@@ -10382,7 +10384,7 @@
         <v>13.69001206862624</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>178</v>
       </c>
@@ -10390,7 +10392,7 @@
         <v>13.711729705516575</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>179</v>
       </c>
@@ -10398,7 +10400,7 @@
         <v>13.756590648161922</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>180</v>
       </c>
@@ -10406,7 +10408,7 @@
         <v>13.827307334701244</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>181</v>
       </c>
@@ -10414,7 +10416,7 @@
         <v>14.036875507054997</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>182</v>
       </c>
@@ -10422,7 +10424,7 @@
         <v>14.53551003872194</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>183</v>
       </c>
@@ -10430,7 +10432,7 @@
         <v>14.68442856810656</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>184</v>
       </c>
@@ -10438,7 +10440,7 @@
         <v>14.85251499938988</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>185</v>
       </c>
@@ -10446,7 +10448,7 @@
         <v>14.869998210726013</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>186</v>
       </c>
@@ -10454,7 +10456,7 @@
         <v>15.022201901472801</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>187</v>
       </c>
@@ -10462,7 +10464,7 @@
         <v>15.108317824582702</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>188</v>
       </c>
@@ -10470,7 +10472,7 @@
         <v>15.123515218219122</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>189</v>
       </c>
@@ -10478,7 +10480,7 @@
         <v>15.235095400808651</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>190</v>
       </c>
@@ -10486,7 +10488,7 @@
         <v>15.518370080345576</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>191</v>
       </c>
@@ -10494,7 +10496,7 @@
         <v>15.892875200460765</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>192</v>
       </c>
@@ -10502,7 +10504,7 @@
         <v>16.172666574789307</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>193</v>
       </c>
@@ -10510,7 +10512,7 @@
         <v>16.279016952537095</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>194</v>
       </c>
@@ -10518,7 +10520,7 @@
         <v>16.332701609445206</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>195</v>
       </c>
@@ -10526,7 +10528,7 @@
         <v>16.360901632623758</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>196</v>
       </c>
@@ -10534,7 +10536,7 @@
         <v>16.622082723269589</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>197</v>
       </c>
@@ -10542,7 +10544,7 @@
         <v>16.664888188921974</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>198</v>
       </c>
@@ -10550,7 +10552,7 @@
         <v>17.126087373353986</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>199</v>
       </c>
@@ -10558,7 +10560,7 @@
         <v>17.216055939380926</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>200</v>
       </c>
@@ -10566,7 +10568,7 @@
         <v>17.324271536888908</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>201</v>
       </c>
@@ -10574,7 +10576,7 @@
         <v>17.526381136816291</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>202</v>
       </c>
@@ -10582,7 +10584,7 @@
         <v>17.559881306464973</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>203</v>
       </c>
@@ -10590,7 +10592,7 @@
         <v>17.971008099871092</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>204</v>
       </c>
@@ -10598,7 +10600,7 @@
         <v>18.204315111929972</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>205</v>
       </c>
@@ -10606,7 +10608,7 @@
         <v>18.844080642498515</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>206</v>
       </c>
@@ -10614,7 +10616,7 @@
         <v>19.114518181232604</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>207</v>
       </c>
@@ -10622,7 +10624,7 @@
         <v>19.480165230844172</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>208</v>
       </c>
@@ -10630,7 +10632,7 @@
         <v>19.758016157724402</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>209</v>
       </c>
@@ -10638,7 +10640,7 @@
         <v>19.780650492844064</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>210</v>
       </c>
@@ -10646,7 +10648,7 @@
         <v>20.201838905921143</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>211</v>
       </c>
@@ -10654,7 +10656,7 @@
         <v>20.35107577461488</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>212</v>
       </c>
@@ -10662,7 +10664,7 @@
         <v>20.449089029758198</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>213</v>
       </c>
@@ -10670,7 +10672,7 @@
         <v>20.61037891270038</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>214</v>
       </c>
@@ -10678,7 +10680,7 @@
         <v>20.792087014352614</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>215</v>
       </c>
@@ -10686,7 +10688,7 @@
         <v>20.831918300314648</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>216</v>
       </c>
@@ -10694,7 +10696,7 @@
         <v>20.881272735680994</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>217</v>
       </c>
@@ -10702,7 +10704,7 @@
         <v>20.924707842433822</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>218</v>
       </c>
@@ -10710,7 +10712,7 @@
         <v>20.926686743324389</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>219</v>
       </c>
@@ -10718,7 +10720,7 @@
         <v>20.927693221638112</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>220</v>
       </c>
@@ -10726,7 +10728,7 @@
         <v>20.947094081371404</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>221</v>
       </c>
@@ -10734,7 +10736,7 @@
         <v>20.97194320982528</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>222</v>
       </c>
@@ -10742,7 +10744,7 @@
         <v>21.236570173683205</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>223</v>
       </c>
@@ -10750,7 +10752,7 @@
         <v>21.270898615511989</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>224</v>
       </c>
@@ -10758,7 +10760,7 @@
         <v>21.417373807782081</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>225</v>
       </c>
@@ -10766,7 +10768,7 @@
         <v>21.762788502146996</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>226</v>
       </c>
@@ -10774,7 +10776,7 @@
         <v>21.844052229155949</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>227</v>
       </c>
@@ -10782,7 +10784,7 @@
         <v>21.862649211279091</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>228</v>
       </c>
@@ -10790,7 +10792,7 @@
         <v>21.921641643182955</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>229</v>
       </c>
@@ -10798,7 +10800,7 @@
         <v>22.043132239478584</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>230</v>
       </c>
@@ -10806,7 +10808,7 @@
         <v>22.225718444421769</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>231</v>
       </c>
@@ -10814,7 +10816,7 @@
         <v>22.270201863023132</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>232</v>
       </c>
@@ -10822,7 +10824,7 @@
         <v>22.657509144081796</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>233</v>
       </c>
@@ -10830,7 +10832,7 @@
         <v>22.717429253394688</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>234</v>
       </c>
@@ -10838,7 +10840,7 @@
         <v>22.790339430280063</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>235</v>
       </c>
@@ -10846,7 +10848,7 @@
         <v>22.925001407787132</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>236</v>
       </c>
@@ -10854,7 +10856,7 @@
         <v>22.939223132457499</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>237</v>
       </c>
@@ -10862,7 +10864,7 @@
         <v>23.067432060092834</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>238</v>
       </c>
@@ -10870,7 +10872,7 @@
         <v>23.070405157587267</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>239</v>
       </c>
@@ -10878,7 +10880,7 @@
         <v>23.350266101241942</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>240</v>
       </c>
@@ -10886,7 +10888,7 @@
         <v>24.240434840233725</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>241</v>
       </c>
@@ -10894,7 +10896,7 @@
         <v>24.380691157218813</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>242</v>
       </c>
@@ -10902,7 +10904,7 @@
         <v>24.59608852779537</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>243</v>
       </c>
@@ -10910,7 +10912,7 @@
         <v>24.767110594901013</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>244</v>
       </c>
@@ -10918,7 +10920,7 @@
         <v>24.821475549560645</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>245</v>
       </c>
@@ -10926,7 +10928,7 @@
         <v>24.86261860734739</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>246</v>
       </c>
@@ -10934,7 +10936,7 @@
         <v>24.866702202641903</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>247</v>
       </c>
@@ -10942,7 +10944,7 @@
         <v>25.479982791216198</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>248</v>
       </c>
@@ -10950,7 +10952,7 @@
         <v>26.239051646786574</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>249</v>
       </c>
@@ -10958,7 +10960,7 @@
         <v>26.620825155605701</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>250</v>
       </c>
@@ -10966,7 +10968,7 @@
         <v>26.660522461733333</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>251</v>
       </c>
@@ -10974,7 +10976,7 @@
         <v>26.717007882651117</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>252</v>
       </c>
@@ -10982,7 +10984,7 @@
         <v>27.073135518125639</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>253</v>
       </c>
@@ -10990,7 +10992,7 @@
         <v>27.416323145371834</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>254</v>
       </c>
@@ -10998,7 +11000,7 @@
         <v>27.453723143857545</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>255</v>
       </c>
@@ -11006,7 +11008,7 @@
         <v>27.618422869970189</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>256</v>
       </c>
@@ -11014,7 +11016,7 @@
         <v>28.054075210901726</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>257</v>
       </c>
@@ -11022,7 +11024,7 @@
         <v>28.349128139480356</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>258</v>
       </c>
@@ -11030,7 +11032,7 @@
         <v>28.422064838288605</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>259</v>
       </c>
@@ -11038,7 +11040,7 @@
         <v>28.640291767656926</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>260</v>
       </c>
@@ -11046,7 +11048,7 @@
         <v>28.671793978080302</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>261</v>
       </c>
@@ -11054,7 +11056,7 @@
         <v>28.675489202000982</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>262</v>
       </c>
@@ -11062,7 +11064,7 @@
         <v>28.785246602101996</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>263</v>
       </c>
@@ -11070,7 +11072,7 @@
         <v>28.847811376909782</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>264</v>
       </c>
@@ -11078,7 +11080,7 @@
         <v>28.928488680724563</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>265</v>
       </c>
@@ -11086,7 +11088,7 @@
         <v>28.92962153717912</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>266</v>
       </c>
@@ -11094,7 +11096,7 @@
         <v>28.973044192765283</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>267</v>
       </c>
@@ -11102,7 +11104,7 @@
         <v>29.469453435657837</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>268</v>
       </c>
@@ -11110,7 +11112,7 @@
         <v>29.666321751336135</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>269</v>
       </c>
@@ -11118,7 +11120,7 @@
         <v>29.815782032049114</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>270</v>
       </c>
@@ -11126,7 +11128,7 @@
         <v>30.035788332456494</v>
       </c>
     </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>271</v>
       </c>
@@ -11134,7 +11136,7 @@
         <v>30.112482402610254</v>
       </c>
     </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>272</v>
       </c>
@@ -11142,7 +11144,7 @@
         <v>30.211163215410785</v>
       </c>
     </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>273</v>
       </c>
@@ -11150,7 +11152,7 @@
         <v>31.239947742766482</v>
       </c>
     </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>274</v>
       </c>
@@ -11158,7 +11160,7 @@
         <v>31.606884891513062</v>
       </c>
     </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>275</v>
       </c>
@@ -11166,7 +11168,7 @@
         <v>31.669765845338084</v>
       </c>
     </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>276</v>
       </c>
@@ -11174,7 +11176,7 @@
         <v>31.771928908088931</v>
       </c>
     </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>277</v>
       </c>
@@ -11182,7 +11184,7 @@
         <v>31.840761444840005</v>
       </c>
     </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>278</v>
       </c>
@@ -11190,7 +11192,7 @@
         <v>32.01918767181094</v>
       </c>
     </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>279</v>
       </c>
@@ -11198,7 +11200,7 @@
         <v>32.075737355475411</v>
       </c>
     </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>280</v>
       </c>
@@ -11206,7 +11208,7 @@
         <v>32.21437505678233</v>
       </c>
     </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>281</v>
       </c>
@@ -11214,7 +11216,7 @@
         <v>32.341321498224183</v>
       </c>
     </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>282</v>
       </c>
@@ -11222,7 +11224,7 @@
         <v>32.376545385017835</v>
       </c>
     </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>283</v>
       </c>
@@ -11230,7 +11232,7 @@
         <v>32.486072733754085</v>
       </c>
     </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>284</v>
       </c>
@@ -11238,7 +11240,7 @@
         <v>32.865144688621776</v>
       </c>
     </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>285</v>
       </c>
@@ -11246,7 +11248,7 @@
         <v>33.015030831623449</v>
       </c>
     </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>286</v>
       </c>
@@ -11254,7 +11256,7 @@
         <v>33.647793837173602</v>
       </c>
     </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>287</v>
       </c>
@@ -11262,7 +11264,7 @@
         <v>34.209172714636978</v>
       </c>
     </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>288</v>
       </c>
@@ -11270,7 +11272,7 @@
         <v>34.21506484295795</v>
       </c>
     </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>289</v>
       </c>
@@ -11278,7 +11280,7 @@
         <v>34.40477991911807</v>
       </c>
     </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>290</v>
       </c>
@@ -11286,7 +11288,7 @@
         <v>34.869240233340527</v>
       </c>
     </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>291</v>
       </c>
@@ -11294,7 +11296,7 @@
         <v>35.857329849769016</v>
       </c>
     </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>292</v>
       </c>
@@ -11302,7 +11304,7 @@
         <v>36.254631666230196</v>
       </c>
     </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>293</v>
       </c>
@@ -11310,7 +11312,7 @@
         <v>36.277466148482731</v>
       </c>
     </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>294</v>
       </c>
@@ -11318,7 +11320,7 @@
         <v>36.610263426063355</v>
       </c>
     </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>295</v>
       </c>
@@ -11326,7 +11328,7 @@
         <v>37.228685106681439</v>
       </c>
     </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>296</v>
       </c>
@@ -11334,7 +11336,7 @@
         <v>37.675183257860397</v>
       </c>
     </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>297</v>
       </c>
@@ -11342,7 +11344,7 @@
         <v>37.732414056487499</v>
       </c>
     </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>298</v>
       </c>
@@ -11350,7 +11352,7 @@
         <v>38.064867410421684</v>
       </c>
     </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>299</v>
       </c>
@@ -11358,7 +11360,7 @@
         <v>38.180590153543037</v>
       </c>
     </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>300</v>
       </c>
@@ -11366,7 +11368,7 @@
         <v>38.387278727877636</v>
       </c>
     </row>
-    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>301</v>
       </c>
@@ -11374,7 +11376,7 @@
         <v>38.9126881761958</v>
       </c>
     </row>
-    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>302</v>
       </c>
@@ -11382,7 +11384,7 @@
         <v>39.03705817021936</v>
       </c>
     </row>
-    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>303</v>
       </c>
@@ -11390,7 +11392,7 @@
         <v>39.136328598605104</v>
       </c>
     </row>
-    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>304</v>
       </c>
@@ -11398,7 +11400,7 @@
         <v>39.554217957038119</v>
       </c>
     </row>
-    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>305</v>
       </c>
@@ -11406,7 +11408,7 @@
         <v>39.978342727275418</v>
       </c>
     </row>
-    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>306</v>
       </c>
@@ -11414,7 +11416,7 @@
         <v>40.085221132529455</v>
       </c>
     </row>
-    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>307</v>
       </c>
@@ -11422,7 +11424,7 @@
         <v>40.265426649196307</v>
       </c>
     </row>
-    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>308</v>
       </c>
@@ -11430,7 +11432,7 @@
         <v>40.289881888279986</v>
       </c>
     </row>
-    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>309</v>
       </c>
@@ -11438,7 +11440,7 @@
         <v>40.454535435984518</v>
       </c>
     </row>
-    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>310</v>
       </c>
@@ -11446,7 +11448,7 @@
         <v>40.654726589364472</v>
       </c>
     </row>
-    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>311</v>
       </c>
@@ -11454,7 +11456,7 @@
         <v>40.823570387135419</v>
       </c>
     </row>
-    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>312</v>
       </c>
@@ -11462,7 +11464,7 @@
         <v>41.192417233278285</v>
       </c>
     </row>
-    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>313</v>
       </c>
@@ -11470,7 +11472,7 @@
         <v>41.276707900560943</v>
       </c>
     </row>
-    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>314</v>
       </c>
@@ -11478,7 +11480,7 @@
         <v>41.409607430918491</v>
       </c>
     </row>
-    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>315</v>
       </c>
@@ -11486,7 +11488,7 @@
         <v>41.972235199258925</v>
       </c>
     </row>
-    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>316</v>
       </c>
@@ -11494,7 +11496,7 @@
         <v>42.12955265826394</v>
       </c>
     </row>
-    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>317</v>
       </c>
@@ -11502,7 +11504,7 @@
         <v>42.142743563271466</v>
       </c>
     </row>
-    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>318</v>
       </c>
@@ -11510,7 +11512,7 @@
         <v>42.213456084822802</v>
       </c>
     </row>
-    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>319</v>
       </c>
@@ -11518,7 +11520,7 @@
         <v>43.693659843636723</v>
       </c>
     </row>
-    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>320</v>
       </c>
@@ -11526,7 +11528,7 @@
         <v>45.3338957634572</v>
       </c>
     </row>
-    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>321</v>
       </c>
@@ -11534,7 +11536,7 @@
         <v>45.79666700836529</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>322</v>
       </c>
@@ -11542,7 +11544,7 @@
         <v>46.047719187309902</v>
       </c>
     </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>323</v>
       </c>
@@ -11550,7 +11552,7 @@
         <v>46.094917449515918</v>
       </c>
     </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>324</v>
       </c>
@@ -11558,7 +11560,7 @@
         <v>46.520409749389977</v>
       </c>
     </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>325</v>
       </c>
@@ -11566,7 +11568,7 @@
         <v>46.587569814693389</v>
       </c>
     </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>326</v>
       </c>
@@ -11574,7 +11576,7 @@
         <v>48.082070951606035</v>
       </c>
     </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>327</v>
       </c>
@@ -11582,7 +11584,7 @@
         <v>48.409060755083956</v>
       </c>
     </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>328</v>
       </c>
@@ -11590,7 +11592,7 @@
         <v>49.047953513158632</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>329</v>
       </c>
@@ -11598,7 +11600,7 @@
         <v>49.466289247640923</v>
       </c>
     </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>330</v>
       </c>
@@ -11606,7 +11608,7 @@
         <v>49.692829116398578</v>
       </c>
     </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>331</v>
       </c>
@@ -11614,7 +11616,7 @@
         <v>49.98166401772081</v>
       </c>
     </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>332</v>
       </c>
@@ -11622,7 +11624,7 @@
         <v>50.098439872183498</v>
       </c>
     </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>333</v>
       </c>
@@ -11630,7 +11632,7 @@
         <v>50.105871701313774</v>
       </c>
     </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>334</v>
       </c>
@@ -11638,7 +11640,7 @@
         <v>50.273612618950722</v>
       </c>
     </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>335</v>
       </c>
@@ -11646,7 +11648,7 @@
         <v>50.310674334274864</v>
       </c>
     </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>336</v>
       </c>
@@ -11654,7 +11656,7 @@
         <v>51.015790941698533</v>
       </c>
     </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>337</v>
       </c>
@@ -11662,7 +11664,7 @@
         <v>51.46946547168767</v>
       </c>
     </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>338</v>
       </c>
@@ -11670,7 +11672,7 @@
         <v>51.749467038151607</v>
       </c>
     </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>339</v>
       </c>
@@ -11678,7 +11680,7 @@
         <v>52.513815224693161</v>
       </c>
     </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>340</v>
       </c>
@@ -11686,7 +11688,7 @@
         <v>52.896124274095264</v>
       </c>
     </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>341</v>
       </c>
@@ -11694,7 +11696,7 @@
         <v>53.724908342578289</v>
       </c>
     </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>342</v>
       </c>
@@ -11702,7 +11704,7 @@
         <v>54.770923310027904</v>
       </c>
     </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>343</v>
       </c>
@@ -11710,7 +11712,7 @@
         <v>55.463694636734914</v>
       </c>
     </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>344</v>
       </c>
@@ -11718,7 +11720,7 @@
         <v>57.463694183097459</v>
       </c>
     </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>345</v>
       </c>
@@ -11726,7 +11728,7 @@
         <v>57.467258590136041</v>
       </c>
     </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>346</v>
       </c>
@@ -11734,7 +11736,7 @@
         <v>59.362696772102161</v>
       </c>
     </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>347</v>
       </c>
@@ -11742,7 +11744,7 @@
         <v>60.550069498372395</v>
       </c>
     </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>348</v>
       </c>
@@ -11750,7 +11752,7 @@
         <v>61.303840990696202</v>
       </c>
     </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>349</v>
       </c>
@@ -11758,7 +11760,7 @@
         <v>61.722392968273645</v>
       </c>
     </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>350</v>
       </c>
@@ -11766,7 +11768,7 @@
         <v>62.452099428444825</v>
       </c>
     </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>351</v>
       </c>
@@ -11774,7 +11776,7 @@
         <v>66.280865071682186</v>
       </c>
     </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A353">
         <v>352</v>
       </c>
@@ -11782,7 +11784,7 @@
         <v>67.257244733515321</v>
       </c>
     </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A354">
         <v>353</v>
       </c>
@@ -11790,7 +11792,7 @@
         <v>75.219929801800419</v>
       </c>
     </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A355">
         <v>354</v>
       </c>
@@ -11798,7 +11800,7 @@
         <v>79.203997428477791</v>
       </c>
     </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A356">
         <v>355</v>
       </c>
@@ -11806,7 +11808,7 @@
         <v>82.001764872280845</v>
       </c>
     </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A357">
         <v>356</v>
       </c>
@@ -11814,7 +11816,7 @@
         <v>83.195200814577035</v>
       </c>
     </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A358">
         <v>357</v>
       </c>
@@ -11822,7 +11824,7 @@
         <v>89.674530555585008</v>
       </c>
     </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A359">
         <v>358</v>
       </c>
@@ -11830,7 +11832,7 @@
         <v>91.0363187291901</v>
       </c>
     </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A360">
         <v>359</v>
       </c>
@@ -11838,7 +11840,7 @@
         <v>93.922980783121872</v>
       </c>
     </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A361">
         <v>360</v>
       </c>
@@ -11846,7 +11848,7 @@
         <v>94.489781152559743</v>
       </c>
     </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A362">
         <v>361</v>
       </c>
@@ -11854,7 +11856,7 @@
         <v>102.09323668814849</v>
       </c>
     </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A363">
         <v>362</v>
       </c>
@@ -11862,7 +11864,7 @@
         <v>112.81560880057754</v>
       </c>
     </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A364">
         <v>363</v>
       </c>
@@ -11870,7 +11872,7 @@
         <v>119.85312233477069</v>
       </c>
     </row>
-    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A365">
         <v>364</v>
       </c>
@@ -11878,7 +11880,7 @@
         <v>128.74511332423194</v>
       </c>
     </row>
-    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A366">
         <v>365</v>
       </c>

</xml_diff>